<commit_message>
Still working on tut1
</commit_message>
<xml_diff>
--- a/ch4-spreadsheets/res/tut1_working.xlsx
+++ b/ch4-spreadsheets/res/tut1_working.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="9900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>We Got Widgets</t>
   </si>
@@ -79,14 +79,44 @@
   </si>
   <si>
     <t>42364</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Glossy</t>
+  </si>
+  <si>
+    <t>rockwell retro encabulator</t>
+  </si>
+  <si>
+    <t>BARCODE</t>
+  </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>FINISH</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>WIDGET</t>
+  </si>
+  <si>
+    <t>7276-86434</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -117,15 +147,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -468,7 +499,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>42964</v>
       </c>
     </row>
@@ -481,7 +512,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -489,26 +520,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -516,7 +550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -524,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -532,7 +566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -540,15 +574,187 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3">
+        <v>12.45</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3">
+        <v>12.45</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3">
+        <v>12.45</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3">
+        <v>12.45</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3">
+        <v>12.45</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on ex 1.2
</commit_message>
<xml_diff>
--- a/ch4-spreadsheets/res/tut1_working.xlsx
+++ b/ch4-spreadsheets/res/tut1_working.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\libraries\Documents\GitHub\computer-apps-primer\ch4-spreadsheets\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\computer-apps-primer\ch4-spreadsheets\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="9900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="9900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>We Got Widgets</t>
   </si>
@@ -148,12 +148,15 @@
   </si>
   <si>
     <t>Wood</t>
+  </si>
+  <si>
+    <t>COST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -511,7 +514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -561,11 +564,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +666,9 @@
       <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,7 +690,10 @@
       <c r="F11" s="3">
         <v>4</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="5">
+        <f>F11*E11</f>
+        <v>49.8</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working on excel tutorial 1.2
</commit_message>
<xml_diff>
--- a/ch4-spreadsheets/res/tut1_working.xlsx
+++ b/ch4-spreadsheets/res/tut1_working.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\computer-apps-primer\ch4-spreadsheets\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\libraries\Documents\GitHub\computer-apps-primer\ch4-spreadsheets\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="9900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>We Got Widgets</t>
   </si>
@@ -151,12 +151,15 @@
   </si>
   <si>
     <t>COST</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -514,7 +517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -564,11 +567,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +718,10 @@
       <c r="F12" s="3">
         <v>2</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="5">
+        <f t="shared" ref="G12:G15" si="0">F12*E12</f>
+        <v>134.9</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -737,7 +743,10 @@
       <c r="F13" s="3">
         <v>16</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>319.83999999999997</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -759,7 +768,10 @@
       <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>8.75</v>
+      </c>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -781,7 +793,10 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>123.4</v>
+      </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -790,8 +805,13 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="5">
+        <f>SUM(G11:G15)</f>
+        <v>636.68999999999994</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ALmost done with Excel tut
</commit_message>
<xml_diff>
--- a/ch4-spreadsheets/res/tut1_working.xlsx
+++ b/ch4-spreadsheets/res/tut1_working.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>We Got Widgets</t>
   </si>
@@ -154,13 +154,26 @@
   </si>
   <si>
     <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Sales Tax</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -193,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -204,6 +217,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,11 +583,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -646,11 +659,15 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.05</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -820,12 +837,32 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="5">
+        <f>G16*G9</f>
+        <v>31.834499999999998</v>
+      </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="7">
+        <v>45</v>
+      </c>
       <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="5">
+        <f>SUM(G16:G18)</f>
+        <v>713.52449999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
almost done with excel tut1-2
</commit_message>
<xml_diff>
--- a/ch4-spreadsheets/res/tut1_working.xlsx
+++ b/ch4-spreadsheets/res/tut1_working.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>We Got Widgets</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>1423-4667</t>
+  </si>
+  <si>
+    <t>Clean</t>
+  </si>
+  <si>
+    <t>capacitive diractants</t>
   </si>
 </sst>
 </file>
@@ -177,9 +186,16 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -194,7 +210,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -202,11 +218,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -215,10 +259,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,289 +631,324 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I19"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G10" s="9">
         <v>0.05</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="10">
         <v>12.45</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F12" s="6">
         <v>4</v>
       </c>
-      <c r="G11" s="5">
-        <f>F11*E11</f>
+      <c r="G12" s="10">
+        <f>F12*E12</f>
         <v>49.8</v>
       </c>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="10">
         <v>67.45</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F13" s="6">
         <v>2</v>
       </c>
-      <c r="G12" s="5">
-        <f t="shared" ref="G12:G15" si="0">F12*E12</f>
+      <c r="G13" s="10">
+        <f t="shared" ref="G13:G17" si="0">F13*E13</f>
         <v>134.9</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="10">
+        <v>45.99</v>
+      </c>
+      <c r="F14" s="6">
+        <v>5</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>229.95000000000002</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E15" s="10">
         <v>19.989999999999998</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F15" s="6">
         <v>16</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G15" s="10">
         <f t="shared" si="0"/>
         <v>319.83999999999997</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E16" s="10">
         <v>8.75</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F16" s="6">
         <v>1</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G16" s="10">
         <f t="shared" si="0"/>
         <v>8.75</v>
       </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E17" s="10">
         <v>123.4</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F17" s="6">
         <v>1</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G17" s="10">
         <f t="shared" si="0"/>
         <v>123.4</v>
       </c>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="5">
-        <f>SUM(G11:G15)</f>
-        <v>636.68999999999994</v>
-      </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
+      <c r="G18" s="10">
+        <f>SUM(G12:G17)</f>
+        <v>866.64</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="5">
-        <f>G16*G9</f>
-        <v>31.834499999999998</v>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
+      <c r="G19" s="10">
+        <f>G18*G10</f>
+        <v>43.332000000000001</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G20" s="11">
         <v>45</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="5">
-        <f>SUM(G16:G18)</f>
-        <v>713.52449999999999</v>
+      <c r="G21" s="10">
+        <f>SUM(G18:G20)</f>
+        <v>954.97199999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>